<commit_message>
Biasing done, first investigations
</commit_message>
<xml_diff>
--- a/results/General Sheet.xlsx
+++ b/results/General Sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11080" windowHeight="0" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11080" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter Investigation" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="90">
   <si>
     <t>Factr Investigation</t>
   </si>
@@ -267,6 +267,30 @@
   </si>
   <si>
     <t>theres ways to test it without having it go to higher dimensions</t>
+  </si>
+  <si>
+    <t>Biasing</t>
+  </si>
+  <si>
+    <t>8k_NNdef_e7_001pi_biastest</t>
+  </si>
+  <si>
+    <t>0 to 1</t>
+  </si>
+  <si>
+    <t>0 to 3/pi</t>
+  </si>
+  <si>
+    <t>0 to 1 no bias</t>
+  </si>
+  <si>
+    <t>8k_NNdef_e7_001pi_biastest2</t>
+  </si>
+  <si>
+    <t>8k_Nndef_e7_001pi_biastest3</t>
+  </si>
+  <si>
+    <t>8k_NNdef_e7_001pi_rangeadjusted</t>
   </si>
 </sst>
 </file>
@@ -527,7 +551,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -607,6 +631,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1793,7 +1820,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -2052,7 +2078,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2444,7 +2469,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -13121,16 +13145,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>562658</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>128607</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>100532</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>494393</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>167144</xdr:rowOff>
+      <xdr:rowOff>110878</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13153,16 +13177,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>533769</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>27377</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>128840</xdr:rowOff>
+      <xdr:rowOff>160992</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>266185</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>587704</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>111926</xdr:rowOff>
+      <xdr:rowOff>144078</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13518,9 +13542,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W92"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14759,97 +14783,279 @@
       <c r="G45" s="20"/>
       <c r="H45" s="20"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="F46" s="38"/>
-      <c r="G46" s="20"/>
-      <c r="H46" s="20"/>
+    <row r="46" spans="1:10" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="63" t="s">
+        <v>82</v>
+      </c>
+      <c r="B46" s="59"/>
+      <c r="C46" s="59"/>
+      <c r="D46" s="59"/>
+      <c r="E46" s="59"/>
+      <c r="F46" s="59"/>
+      <c r="G46" s="59"/>
+      <c r="H46" s="59"/>
+      <c r="I46" s="60"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="F47" s="38"/>
-      <c r="G47" s="20"/>
-      <c r="H47" s="20"/>
+      <c r="A47" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" s="65">
+        <v>8000</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D47" s="18">
+        <v>10000000</v>
+      </c>
+      <c r="E47" s="5">
+        <v>5000</v>
+      </c>
+      <c r="F47" s="29">
+        <v>215.85521507263101</v>
+      </c>
+      <c r="G47" s="21">
+        <v>2.3937971413045098E-3</v>
+      </c>
+      <c r="H47" s="21">
+        <v>1.4509705023949399E-2</v>
+      </c>
+      <c r="I47" s="7">
+        <v>1.1226E-4</v>
+      </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="F48" s="38"/>
-      <c r="G48" s="20"/>
-      <c r="H48" s="20"/>
+      <c r="A48" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B48" s="66">
+        <v>8000</v>
+      </c>
+      <c r="C48" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D48" s="18">
+        <v>10000000</v>
+      </c>
+      <c r="E48" s="33">
+        <v>5000</v>
+      </c>
+      <c r="F48" s="29">
+        <v>308.12270307540803</v>
+      </c>
+      <c r="G48" s="21">
+        <v>9.4159016988517603E-3</v>
+      </c>
+      <c r="H48" s="21">
+        <v>2.69920616086343E-2</v>
+      </c>
+      <c r="I48" s="7">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="J48" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="49" spans="6:8" x14ac:dyDescent="0.35">
-      <c r="F49" s="38"/>
-      <c r="G49" s="20"/>
-      <c r="H49" s="20"/>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A49" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B49" s="66">
+        <v>8000</v>
+      </c>
+      <c r="C49" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D49" s="18">
+        <v>10000000</v>
+      </c>
+      <c r="E49" s="34">
+        <v>5000</v>
+      </c>
+      <c r="F49" s="29">
+        <v>342.18696832656798</v>
+      </c>
+      <c r="G49" s="21">
+        <v>2.1007359942959401E-3</v>
+      </c>
+      <c r="H49" s="49">
+        <v>9.5780617055238604E-3</v>
+      </c>
+      <c r="I49" s="7">
+        <v>9.5452999999999996E-5</v>
+      </c>
+      <c r="J49" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="50" spans="6:8" x14ac:dyDescent="0.35">
-      <c r="F50" s="38"/>
-      <c r="G50" s="20"/>
-      <c r="H50" s="20"/>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A50" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B50" s="66">
+        <v>8000</v>
+      </c>
+      <c r="C50" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D50" s="18">
+        <v>10000000</v>
+      </c>
+      <c r="E50" s="34">
+        <v>5000</v>
+      </c>
+      <c r="F50" s="54">
+        <v>403.35344457626297</v>
+      </c>
+      <c r="G50" s="49">
+        <v>2.7503100918850002E-3</v>
+      </c>
+      <c r="H50" s="49">
+        <v>1.2097230694490301E-2</v>
+      </c>
+      <c r="I50" s="7">
+        <v>1.039E-4</v>
+      </c>
+      <c r="J50" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="51" spans="6:8" x14ac:dyDescent="0.35">
-      <c r="F51" s="38"/>
-      <c r="G51" s="20"/>
-      <c r="H51" s="20"/>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A51" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="B51" s="66">
+        <v>8000</v>
+      </c>
+      <c r="C51" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D51" s="18">
+        <v>10000000</v>
+      </c>
+      <c r="E51" s="34">
+        <v>5000</v>
+      </c>
+      <c r="F51" s="29">
+        <v>333.25974106788601</v>
+      </c>
+      <c r="G51" s="21">
+        <v>1.4766566504602499E-3</v>
+      </c>
+      <c r="H51" s="21">
+        <v>4.6200240936638097E-3</v>
+      </c>
+      <c r="I51" s="7">
+        <v>1.1613E-4</v>
+      </c>
+      <c r="J51" t="s">
+        <v>86</v>
+      </c>
     </row>
-    <row r="52" spans="6:8" x14ac:dyDescent="0.35">
-      <c r="F52" s="38"/>
-      <c r="G52" s="20"/>
-      <c r="H52" s="20"/>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A52" s="67"/>
+      <c r="B52" s="66"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="29"/>
+      <c r="G52" s="21"/>
+      <c r="H52" s="21"/>
+      <c r="I52" s="7"/>
     </row>
-    <row r="53" spans="6:8" x14ac:dyDescent="0.35">
-      <c r="F53" s="38"/>
-      <c r="G53" s="20"/>
-      <c r="H53" s="20"/>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A53" s="13"/>
+      <c r="B53" s="39"/>
+      <c r="C53" s="17"/>
+      <c r="D53" s="17"/>
+      <c r="E53" s="32"/>
+      <c r="F53" s="28"/>
+      <c r="G53" s="26"/>
+      <c r="H53" s="26"/>
+      <c r="I53" s="16"/>
     </row>
-    <row r="54" spans="6:8" x14ac:dyDescent="0.35">
-      <c r="F54" s="38"/>
-      <c r="G54" s="20"/>
-      <c r="H54" s="20"/>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A54" s="13"/>
+      <c r="B54" s="40"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="33"/>
+      <c r="F54" s="29"/>
+      <c r="G54" s="21"/>
+      <c r="H54" s="21"/>
+      <c r="I54" s="7"/>
     </row>
-    <row r="55" spans="6:8" x14ac:dyDescent="0.35">
-      <c r="F55" s="38"/>
-      <c r="G55" s="20"/>
-      <c r="H55" s="20"/>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A55" s="13"/>
+      <c r="B55" s="40"/>
+      <c r="C55" s="18"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="34"/>
+      <c r="F55" s="29"/>
+      <c r="G55" s="21"/>
+      <c r="H55" s="49"/>
+      <c r="I55" s="7"/>
     </row>
-    <row r="56" spans="6:8" x14ac:dyDescent="0.35">
-      <c r="F56" s="38"/>
-      <c r="G56" s="20"/>
-      <c r="H56" s="20"/>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A56" s="13"/>
+      <c r="B56" s="40"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="34"/>
+      <c r="F56" s="54"/>
+      <c r="G56" s="49"/>
+      <c r="H56" s="49"/>
+      <c r="I56" s="7"/>
     </row>
-    <row r="57" spans="6:8" x14ac:dyDescent="0.35">
-      <c r="F57" s="38"/>
-      <c r="G57" s="20"/>
-      <c r="H57" s="20"/>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A57" s="13"/>
+      <c r="B57" s="40"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="29"/>
+      <c r="G57" s="21"/>
+      <c r="H57" s="21"/>
+      <c r="I57" s="7"/>
     </row>
-    <row r="58" spans="6:8" x14ac:dyDescent="0.35">
-      <c r="F58" s="38"/>
-      <c r="G58" s="20"/>
-      <c r="H58" s="20"/>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A58" s="14"/>
+      <c r="B58" s="45"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="46"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="30"/>
+      <c r="G58" s="24"/>
+      <c r="H58" s="24"/>
+      <c r="I58" s="10"/>
     </row>
-    <row r="59" spans="6:8" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="F59" s="38"/>
       <c r="G59" s="20"/>
       <c r="H59" s="20"/>
     </row>
-    <row r="60" spans="6:8" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="F60" s="38"/>
       <c r="G60" s="20"/>
       <c r="H60" s="20"/>
     </row>
-    <row r="61" spans="6:8" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="F61" s="38"/>
       <c r="G61" s="20"/>
       <c r="H61" s="20"/>
     </row>
-    <row r="62" spans="6:8" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="F62" s="38"/>
       <c r="G62" s="20"/>
       <c r="H62" s="20"/>
     </row>
-    <row r="63" spans="6:8" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="F63" s="38"/>
       <c r="G63" s="20"/>
       <c r="H63" s="20"/>
     </row>
-    <row r="64" spans="6:8" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="F64" s="38"/>
       <c r="G64" s="20"/>
       <c r="H64" s="20"/>
@@ -14975,11 +15181,12 @@
       <c r="F92" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A23:I23"/>
     <mergeCell ref="A11:I11"/>
     <mergeCell ref="A32:I32"/>
+    <mergeCell ref="A46:I46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
@@ -14991,7 +15198,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A272" workbookViewId="0">
+    <sheetView topLeftCell="A272" workbookViewId="0">
       <selection activeCell="I300" sqref="I300"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Autorunner works! Using more complex bias next
</commit_message>
<xml_diff>
--- a/results/General Sheet.xlsx
+++ b/results/General Sheet.xlsx
@@ -785,6 +785,28 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -804,15 +826,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -822,29 +837,14 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -900,7 +900,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1156,7 +1155,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1425,7 +1423,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2343,7 +2340,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>quite arbitrary scale)</a:t>
+                  <a:t>arbitrary scale)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3492,7 +3489,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3981,7 +3977,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4348,7 +4343,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4909,7 +4903,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5018,7 +5011,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5405,7 +5397,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5515,7 +5506,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6249,7 +6239,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6516,7 +6505,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6864,7 +6852,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -14659,8 +14646,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="11962208" y="300626"/>
-          <a:ext cx="9309804" cy="5072153"/>
+          <a:off x="11986871" y="304676"/>
+          <a:ext cx="9345144" cy="5185532"/>
           <a:chOff x="11091396" y="529291"/>
           <a:chExt cx="9392956" cy="5199477"/>
         </a:xfrm>
@@ -14940,50 +14927,6 @@
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>353391</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>88348</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>414130</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>115957</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="15" name="Straight Connector 14"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="17951174" y="452783"/>
-          <a:ext cx="60739" cy="3125304"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -15364,17 +15307,17 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="74"/>
       <c r="J2" t="s">
         <v>11</v>
       </c>
@@ -15590,17 +15533,17 @@
     </row>
     <row r="10" spans="1:23" ht="21.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="11" spans="1:23" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="60" t="s">
+      <c r="A11" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="63"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="63"/>
-      <c r="H11" s="63"/>
-      <c r="I11" s="64"/>
+      <c r="B11" s="75"/>
+      <c r="C11" s="75"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="75"/>
+      <c r="G11" s="75"/>
+      <c r="H11" s="75"/>
+      <c r="I11" s="76"/>
       <c r="J11" t="s">
         <v>43</v>
       </c>
@@ -15935,17 +15878,17 @@
       </c>
     </row>
     <row r="23" spans="1:23" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="60" t="s">
+      <c r="A23" s="72" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="61"/>
-      <c r="C23" s="61"/>
-      <c r="D23" s="61"/>
-      <c r="E23" s="61"/>
-      <c r="F23" s="61"/>
-      <c r="G23" s="61"/>
-      <c r="H23" s="61"/>
-      <c r="I23" s="62"/>
+      <c r="B23" s="73"/>
+      <c r="C23" s="73"/>
+      <c r="D23" s="73"/>
+      <c r="E23" s="73"/>
+      <c r="F23" s="73"/>
+      <c r="G23" s="73"/>
+      <c r="H23" s="73"/>
+      <c r="I23" s="74"/>
       <c r="J23" t="s">
         <v>61</v>
       </c>
@@ -16189,17 +16132,17 @@
       <c r="H31" s="20"/>
     </row>
     <row r="32" spans="1:23" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="60" t="s">
+      <c r="A32" s="72" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="61"/>
-      <c r="C32" s="61"/>
-      <c r="D32" s="61"/>
-      <c r="E32" s="61"/>
-      <c r="F32" s="61"/>
-      <c r="G32" s="61"/>
-      <c r="H32" s="61"/>
-      <c r="I32" s="62"/>
+      <c r="B32" s="73"/>
+      <c r="C32" s="73"/>
+      <c r="D32" s="73"/>
+      <c r="E32" s="73"/>
+      <c r="F32" s="73"/>
+      <c r="G32" s="73"/>
+      <c r="H32" s="73"/>
+      <c r="I32" s="74"/>
       <c r="J32" t="s">
         <v>11</v>
       </c>
@@ -16561,17 +16504,17 @@
       <c r="H45" s="20"/>
     </row>
     <row r="46" spans="1:10" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="65" t="s">
+      <c r="A46" s="77" t="s">
         <v>82</v>
       </c>
-      <c r="B46" s="61"/>
-      <c r="C46" s="61"/>
-      <c r="D46" s="61"/>
-      <c r="E46" s="61"/>
-      <c r="F46" s="61"/>
-      <c r="G46" s="61"/>
-      <c r="H46" s="61"/>
-      <c r="I46" s="62"/>
+      <c r="B46" s="73"/>
+      <c r="C46" s="73"/>
+      <c r="D46" s="73"/>
+      <c r="E46" s="73"/>
+      <c r="F46" s="73"/>
+      <c r="G46" s="73"/>
+      <c r="H46" s="73"/>
+      <c r="I46" s="74"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="55" t="s">
@@ -16906,8 +16849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="75" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="U23" sqref="U23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16920,10 +16863,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="78" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="67"/>
+      <c r="B1" s="78"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -16945,7 +16888,7 @@
       <c r="A4" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="60" t="s">
         <v>39</v>
       </c>
     </row>
@@ -16956,83 +16899,83 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C7" s="70" t="s">
+      <c r="C7" s="79" t="s">
         <v>101</v>
       </c>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="79" t="s">
+      <c r="D7" s="80"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="80"/>
+      <c r="G7" s="80"/>
+      <c r="H7" s="81"/>
+      <c r="I7" s="82" t="s">
         <v>102</v>
       </c>
-      <c r="J7" s="80"/>
-      <c r="K7" s="80"/>
-      <c r="L7" s="80"/>
+      <c r="J7" s="83"/>
+      <c r="K7" s="83"/>
+      <c r="L7" s="83"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C8" s="77" t="s">
+      <c r="C8" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="D8" s="77" t="s">
+      <c r="D8" s="66" t="s">
         <v>95</v>
       </c>
-      <c r="E8" s="77" t="s">
+      <c r="E8" s="66" t="s">
         <v>96</v>
       </c>
-      <c r="F8" s="77" t="s">
+      <c r="F8" s="66" t="s">
         <v>97</v>
       </c>
-      <c r="G8" s="77" t="s">
+      <c r="G8" s="66" t="s">
         <v>135</v>
       </c>
-      <c r="H8" s="77" t="s">
+      <c r="H8" s="66" t="s">
         <v>98</v>
       </c>
-      <c r="I8" s="78" t="s">
+      <c r="I8" s="67" t="s">
         <v>103</v>
       </c>
-      <c r="J8" s="78" t="s">
+      <c r="J8" s="67" t="s">
         <v>104</v>
       </c>
-      <c r="K8" s="78" t="s">
+      <c r="K8" s="67" t="s">
         <v>105</v>
       </c>
-      <c r="L8" s="78" t="s">
+      <c r="L8" s="67" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C9" s="75" t="s">
+      <c r="C9" s="64" t="s">
         <v>111</v>
       </c>
-      <c r="D9" s="75">
+      <c r="D9" s="64">
         <v>8000</v>
       </c>
-      <c r="E9" s="75">
+      <c r="E9" s="64">
         <v>3</v>
       </c>
-      <c r="F9" s="75" t="s">
+      <c r="F9" s="64" t="s">
         <v>110</v>
       </c>
-      <c r="G9" s="75">
+      <c r="G9" s="64">
         <f>5/2.5</f>
         <v>2</v>
       </c>
-      <c r="H9" s="76" t="s">
+      <c r="H9" s="65" t="s">
         <v>106</v>
       </c>
-      <c r="I9" s="74">
+      <c r="I9" s="63">
         <v>260.2</v>
       </c>
-      <c r="J9" s="74">
+      <c r="J9" s="63">
         <v>4.2488640125852304E-3</v>
       </c>
-      <c r="K9" s="74">
+      <c r="K9" s="63">
         <v>2.7196150664271002E-2</v>
       </c>
-      <c r="L9" s="81">
+      <c r="L9" s="68">
         <v>3.0615999999999998E-4</v>
       </c>
       <c r="M9" t="s">
@@ -17040,35 +16983,35 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C10" s="73" t="s">
+      <c r="C10" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="D10" s="73">
+      <c r="D10" s="62">
         <v>8000</v>
       </c>
-      <c r="E10" s="73">
+      <c r="E10" s="62">
         <v>3</v>
       </c>
-      <c r="F10" s="75" t="s">
+      <c r="F10" s="64" t="s">
         <v>110</v>
       </c>
-      <c r="G10" s="75">
+      <c r="G10" s="64">
         <f>6/2</f>
         <v>3</v>
       </c>
-      <c r="H10" s="75" t="s">
+      <c r="H10" s="64" t="s">
         <v>107</v>
       </c>
-      <c r="I10" s="74">
+      <c r="I10" s="63">
         <v>323.67</v>
       </c>
-      <c r="J10" s="74">
+      <c r="J10" s="63">
         <v>1.6072221063274301E-3</v>
       </c>
-      <c r="K10" s="74">
+      <c r="K10" s="63">
         <v>8.0899315411814693E-3</v>
       </c>
-      <c r="L10" s="81">
+      <c r="L10" s="68">
         <v>1.5983999999999999E-4</v>
       </c>
       <c r="M10" t="s">
@@ -17076,71 +17019,71 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C11" s="73" t="s">
+      <c r="C11" s="62" t="s">
         <v>115</v>
       </c>
-      <c r="D11" s="73">
+      <c r="D11" s="62">
         <v>8000</v>
       </c>
-      <c r="E11" s="73">
+      <c r="E11" s="62">
         <v>3</v>
       </c>
-      <c r="F11" s="75" t="s">
+      <c r="F11" s="64" t="s">
         <v>110</v>
       </c>
-      <c r="G11" s="75">
+      <c r="G11" s="64">
         <f>7/1.5</f>
         <v>4.666666666666667</v>
       </c>
-      <c r="H11" s="75" t="s">
+      <c r="H11" s="64" t="s">
         <v>108</v>
       </c>
-      <c r="I11" s="74">
+      <c r="I11" s="63">
         <v>259.76</v>
       </c>
-      <c r="J11" s="74">
+      <c r="J11" s="63">
         <v>1.82242784880268E-3</v>
       </c>
-      <c r="K11" s="74">
+      <c r="K11" s="63">
         <v>8.4242252783167E-3</v>
       </c>
-      <c r="L11" s="81">
+      <c r="L11" s="68">
         <v>7.4729999999999998E-5</v>
       </c>
-      <c r="M11" s="82" t="s">
+      <c r="M11" s="69" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C12" s="73" t="s">
+      <c r="C12" s="62" t="s">
         <v>116</v>
       </c>
-      <c r="D12" s="73">
+      <c r="D12" s="62">
         <v>8000</v>
       </c>
-      <c r="E12" s="73">
+      <c r="E12" s="62">
         <v>3</v>
       </c>
-      <c r="F12" s="75" t="s">
+      <c r="F12" s="64" t="s">
         <v>110</v>
       </c>
-      <c r="G12" s="75">
+      <c r="G12" s="64">
         <f>8/1</f>
         <v>8</v>
       </c>
-      <c r="H12" s="75" t="s">
+      <c r="H12" s="64" t="s">
         <v>109</v>
       </c>
-      <c r="I12" s="74">
+      <c r="I12" s="63">
         <v>323.75642228126497</v>
       </c>
-      <c r="J12" s="74">
+      <c r="J12" s="63">
         <v>7.47970370899868E-3</v>
       </c>
-      <c r="K12" s="74">
+      <c r="K12" s="63">
         <v>2.9637786654420399E-2</v>
       </c>
-      <c r="L12" s="81">
+      <c r="L12" s="68">
         <v>9.2113999999999998E-4</v>
       </c>
       <c r="M12" t="s">
@@ -17148,304 +17091,304 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C13" s="75" t="s">
+      <c r="C13" s="64" t="s">
         <v>99</v>
       </c>
-      <c r="D13" s="73">
+      <c r="D13" s="62">
         <v>8000</v>
       </c>
-      <c r="E13" s="73">
+      <c r="E13" s="62">
         <v>3</v>
       </c>
-      <c r="F13" s="75" t="s">
+      <c r="F13" s="64" t="s">
         <v>119</v>
       </c>
-      <c r="G13" s="75">
+      <c r="G13" s="64">
         <f>5/2.5</f>
         <v>2</v>
       </c>
-      <c r="H13" s="76" t="s">
+      <c r="H13" s="65" t="s">
         <v>123</v>
       </c>
-      <c r="I13" s="74">
+      <c r="I13" s="63">
         <v>302.75013160705498</v>
       </c>
-      <c r="J13" s="74">
+      <c r="J13" s="63">
         <v>2.2049460806415002E-3</v>
       </c>
-      <c r="K13" s="74">
+      <c r="K13" s="63">
         <v>1.13965165096503E-2</v>
       </c>
-      <c r="L13" s="81">
+      <c r="L13" s="68">
         <v>2.2330000000000001E-4</v>
       </c>
-      <c r="M13" s="83" t="s">
+      <c r="M13" s="70" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C14" s="73" t="s">
+      <c r="C14" s="62" t="s">
         <v>100</v>
       </c>
-      <c r="D14" s="73">
+      <c r="D14" s="62">
         <v>8000</v>
       </c>
-      <c r="E14" s="73">
+      <c r="E14" s="62">
         <v>3</v>
       </c>
-      <c r="F14" s="75" t="s">
+      <c r="F14" s="64" t="s">
         <v>120</v>
       </c>
-      <c r="G14" s="75">
+      <c r="G14" s="64">
         <f>6/2</f>
         <v>3</v>
       </c>
-      <c r="H14" s="75" t="s">
+      <c r="H14" s="64" t="s">
         <v>124</v>
       </c>
-      <c r="I14" s="74">
+      <c r="I14" s="63">
         <v>336.44930267333899</v>
       </c>
-      <c r="J14" s="74">
+      <c r="J14" s="63">
         <v>2.5720768185244799E-3</v>
       </c>
-      <c r="K14" s="74">
+      <c r="K14" s="63">
         <v>1.03399548659959E-2</v>
       </c>
-      <c r="L14" s="81">
+      <c r="L14" s="68">
         <v>3.0962999999999997E-4</v>
       </c>
-      <c r="M14" s="83" t="s">
+      <c r="M14" s="70" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C15" s="73" t="s">
+      <c r="C15" s="62" t="s">
         <v>118</v>
       </c>
-      <c r="D15" s="73">
+      <c r="D15" s="62">
         <v>8000</v>
       </c>
-      <c r="E15" s="73">
+      <c r="E15" s="62">
         <v>3</v>
       </c>
-      <c r="F15" s="75" t="s">
+      <c r="F15" s="64" t="s">
         <v>121</v>
       </c>
-      <c r="G15" s="75">
+      <c r="G15" s="64">
         <f>7/1.5</f>
         <v>4.666666666666667</v>
       </c>
-      <c r="H15" s="75" t="s">
+      <c r="H15" s="64" t="s">
         <v>125</v>
       </c>
-      <c r="I15" s="74">
+      <c r="I15" s="63">
         <v>268.47458791732703</v>
       </c>
-      <c r="J15" s="74">
+      <c r="J15" s="63">
         <v>1.8323629909740499E-3</v>
       </c>
-      <c r="K15" s="74">
+      <c r="K15" s="63">
         <v>4.1662992684478499E-3</v>
       </c>
-      <c r="L15" s="81">
+      <c r="L15" s="68">
         <v>1.0760999999999999E-4</v>
       </c>
-      <c r="M15" s="83" t="s">
+      <c r="M15" s="70" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C16" s="73" t="s">
+      <c r="C16" s="62" t="s">
         <v>117</v>
       </c>
-      <c r="D16" s="73">
+      <c r="D16" s="62">
         <v>8000</v>
       </c>
-      <c r="E16" s="73">
+      <c r="E16" s="62">
         <v>3</v>
       </c>
-      <c r="F16" s="75" t="s">
+      <c r="F16" s="64" t="s">
         <v>122</v>
       </c>
-      <c r="G16" s="75">
+      <c r="G16" s="64">
         <f>8/1</f>
         <v>8</v>
       </c>
-      <c r="H16" s="75" t="s">
+      <c r="H16" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="I16" s="74">
+      <c r="I16" s="63">
         <v>308.39033603668202</v>
       </c>
-      <c r="J16" s="74">
+      <c r="J16" s="63">
         <v>2.38427413612335E-3</v>
       </c>
-      <c r="K16" s="74">
+      <c r="K16" s="63">
         <v>6.6410735564910702E-3</v>
       </c>
-      <c r="L16" s="81">
+      <c r="L16" s="68">
         <v>1.4899999999999999E-4</v>
       </c>
-      <c r="M16" s="83" t="s">
+      <c r="M16" s="70" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C17" s="69"/>
-      <c r="D17" s="69"/>
-      <c r="E17" s="69"/>
-      <c r="F17" s="84"/>
-      <c r="G17" s="84"/>
-      <c r="H17" s="84"/>
-      <c r="I17" s="69"/>
-      <c r="J17" s="69"/>
-      <c r="K17" s="69"/>
-      <c r="L17" s="69"/>
+      <c r="C17" s="61"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="71"/>
+      <c r="G17" s="71"/>
+      <c r="H17" s="71"/>
+      <c r="I17" s="61"/>
+      <c r="J17" s="61"/>
+      <c r="K17" s="61"/>
+      <c r="L17" s="61"/>
     </row>
     <row r="18" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C18" s="73" t="s">
+      <c r="C18" s="62" t="s">
         <v>131</v>
       </c>
-      <c r="D18" s="73">
+      <c r="D18" s="62">
         <v>2500</v>
       </c>
-      <c r="E18" s="73">
+      <c r="E18" s="62">
         <v>3</v>
       </c>
-      <c r="F18" s="75" t="s">
+      <c r="F18" s="64" t="s">
         <v>110</v>
       </c>
-      <c r="G18" s="75">
+      <c r="G18" s="64">
         <f>5/2.5</f>
         <v>2</v>
       </c>
-      <c r="H18" s="76" t="s">
+      <c r="H18" s="65" t="s">
         <v>106</v>
       </c>
-      <c r="I18" s="74">
+      <c r="I18" s="63">
         <v>109.93222713470399</v>
       </c>
-      <c r="J18" s="74">
+      <c r="J18" s="63">
         <v>1.7201413965715399E-2</v>
       </c>
-      <c r="K18" s="74">
+      <c r="K18" s="63">
         <v>0.11805720295071299</v>
       </c>
-      <c r="L18" s="81">
+      <c r="L18" s="68">
         <v>1.6752999999999999E-4</v>
       </c>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C19" s="73" t="s">
+      <c r="C19" s="62" t="s">
         <v>132</v>
       </c>
-      <c r="D19" s="73">
+      <c r="D19" s="62">
         <v>2500</v>
       </c>
-      <c r="E19" s="73">
+      <c r="E19" s="62">
         <v>3</v>
       </c>
-      <c r="F19" s="75" t="s">
+      <c r="F19" s="64" t="s">
         <v>110</v>
       </c>
-      <c r="G19" s="75">
+      <c r="G19" s="64">
         <f>6/2</f>
         <v>3</v>
       </c>
-      <c r="H19" s="75" t="s">
+      <c r="H19" s="64" t="s">
         <v>107</v>
       </c>
-      <c r="I19" s="74">
+      <c r="I19" s="63">
         <v>99.864153623580904</v>
       </c>
-      <c r="J19" s="74">
+      <c r="J19" s="63">
         <v>1.0163619445984699E-2</v>
       </c>
-      <c r="K19" s="74">
+      <c r="K19" s="63">
         <v>6.01173925445855E-2</v>
       </c>
-      <c r="L19" s="81">
+      <c r="L19" s="68">
         <v>2.7883999999999998E-4</v>
       </c>
     </row>
     <row r="20" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C20" s="73" t="s">
+      <c r="C20" s="62" t="s">
         <v>133</v>
       </c>
-      <c r="D20" s="73">
+      <c r="D20" s="62">
         <v>2500</v>
       </c>
-      <c r="E20" s="73">
+      <c r="E20" s="62">
         <v>3</v>
       </c>
-      <c r="F20" s="75" t="s">
+      <c r="F20" s="64" t="s">
         <v>110</v>
       </c>
-      <c r="G20" s="75">
+      <c r="G20" s="64">
         <f>7/1.5</f>
         <v>4.666666666666667</v>
       </c>
-      <c r="H20" s="75" t="s">
+      <c r="H20" s="64" t="s">
         <v>108</v>
       </c>
-      <c r="I20" s="74">
+      <c r="I20" s="63">
         <v>101.51741313934301</v>
       </c>
-      <c r="J20" s="74">
+      <c r="J20" s="63">
         <v>3.6305701878396701E-3</v>
       </c>
-      <c r="K20" s="74">
+      <c r="K20" s="63">
         <v>2.3130133244623902E-2</v>
       </c>
-      <c r="L20" s="81">
+      <c r="L20" s="68">
         <v>6.7063999999999994E-5</v>
       </c>
     </row>
     <row r="21" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C21" s="73" t="s">
+      <c r="C21" s="62" t="s">
         <v>134</v>
       </c>
-      <c r="D21" s="73">
+      <c r="D21" s="62">
         <v>2500</v>
       </c>
-      <c r="E21" s="73">
+      <c r="E21" s="62">
         <v>3</v>
       </c>
-      <c r="F21" s="75" t="s">
+      <c r="F21" s="64" t="s">
         <v>110</v>
       </c>
-      <c r="G21" s="75">
+      <c r="G21" s="64">
         <f>8/1</f>
         <v>8</v>
       </c>
-      <c r="H21" s="75" t="s">
+      <c r="H21" s="64" t="s">
         <v>109</v>
       </c>
-      <c r="I21" s="74">
+      <c r="I21" s="63">
         <v>118.18180060386599</v>
       </c>
-      <c r="J21" s="74">
+      <c r="J21" s="63">
         <v>7.0018257112560304E-3</v>
       </c>
-      <c r="K21" s="74">
+      <c r="K21" s="63">
         <v>4.7148616969688598E-2</v>
       </c>
-      <c r="L21" s="81">
+      <c r="L21" s="68">
         <v>1.1417999999999999E-4</v>
       </c>
     </row>
     <row r="22" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C22" s="73"/>
-      <c r="D22" s="73"/>
-      <c r="E22" s="73"/>
-      <c r="F22" s="75"/>
-      <c r="G22" s="75"/>
-      <c r="H22" s="75"/>
-      <c r="I22" s="74"/>
-      <c r="J22" s="74"/>
-      <c r="K22" s="74"/>
-      <c r="L22" s="74"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="62"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="64"/>
+      <c r="G22" s="64"/>
+      <c r="H22" s="64"/>
+      <c r="I22" s="63"/>
+      <c r="J22" s="63"/>
+      <c r="K22" s="63"/>
+      <c r="L22" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -17720,13 +17663,13 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:19" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="63"/>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="64"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="76"/>
       <c r="F4" t="s">
         <v>11</v>
       </c>
@@ -17878,12 +17821,12 @@
       <c r="A12" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="P12" s="66" t="s">
+      <c r="P12" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="Q12" s="66"/>
-      <c r="R12" s="66"/>
-      <c r="S12" s="66"/>
+      <c r="Q12" s="84"/>
+      <c r="R12" s="84"/>
+      <c r="S12" s="84"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
@@ -17904,10 +17847,10 @@
       <c r="F13" s="16">
         <v>2.8798000000000001E-5</v>
       </c>
-      <c r="P13" s="66"/>
-      <c r="Q13" s="66"/>
-      <c r="R13" s="66"/>
-      <c r="S13" s="66"/>
+      <c r="P13" s="84"/>
+      <c r="Q13" s="84"/>
+      <c r="R13" s="84"/>
+      <c r="S13" s="84"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14" s="13" t="s">
@@ -17929,10 +17872,10 @@
       <c r="F14" s="7">
         <v>1.058E-4</v>
       </c>
-      <c r="P14" s="66"/>
-      <c r="Q14" s="66"/>
-      <c r="R14" s="66"/>
-      <c r="S14" s="66"/>
+      <c r="P14" s="84"/>
+      <c r="Q14" s="84"/>
+      <c r="R14" s="84"/>
+      <c r="S14" s="84"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15" s="13" t="s">
@@ -17952,10 +17895,10 @@
         <v>8.7702261052175406E-2</v>
       </c>
       <c r="F15" s="6"/>
-      <c r="P15" s="66"/>
-      <c r="Q15" s="66"/>
-      <c r="R15" s="66"/>
-      <c r="S15" s="66"/>
+      <c r="P15" s="84"/>
+      <c r="Q15" s="84"/>
+      <c r="R15" s="84"/>
+      <c r="S15" s="84"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16" s="14" t="s">
@@ -17977,19 +17920,19 @@
       <c r="F16" s="10">
         <v>1.1573000000000001E-5</v>
       </c>
-      <c r="P16" s="66"/>
-      <c r="Q16" s="66"/>
-      <c r="R16" s="66"/>
-      <c r="S16" s="66"/>
+      <c r="P16" s="84"/>
+      <c r="Q16" s="84"/>
+      <c r="R16" s="84"/>
+      <c r="S16" s="84"/>
     </row>
     <row r="18" spans="1:5" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="65" t="s">
+      <c r="A18" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="63"/>
-      <c r="C18" s="63"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="64"/>
+      <c r="B18" s="75"/>
+      <c r="C18" s="75"/>
+      <c r="D18" s="75"/>
+      <c r="E18" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Autorunning works... Must check error calculation
</commit_message>
<xml_diff>
--- a/results/General Sheet.xlsx
+++ b/results/General Sheet.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11080" windowHeight="0" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11080" windowHeight="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter Investigation" sheetId="3" r:id="rId1"/>
     <sheet name="Bias Investigation" sheetId="4" r:id="rId2"/>
-    <sheet name="FDM" sheetId="2" r:id="rId3"/>
-    <sheet name="old investigation" sheetId="1" r:id="rId4"/>
+    <sheet name="Type2Bias" sheetId="5" r:id="rId3"/>
+    <sheet name="FDM" sheetId="2" r:id="rId4"/>
+    <sheet name="old investigation" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="139">
   <si>
     <t>Factr Investigation</t>
   </si>
@@ -431,6 +432,15 @@
   <si>
     <t>???</t>
   </si>
+  <si>
+    <t>pt1</t>
+  </si>
+  <si>
+    <t>xdiv</t>
+  </si>
+  <si>
+    <t>case0</t>
+  </si>
 </sst>
 </file>
 
@@ -724,7 +734,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -846,6 +856,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -900,6 +913,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1155,6 +1169,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1423,6 +1438,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3489,6 +3505,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3977,6 +3994,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4343,6 +4361,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6239,6 +6258,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6505,6 +6525,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6852,6 +6873,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -16849,8 +16871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="75" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="U23" sqref="U23"/>
+    <sheetView zoomScale="75" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17404,6 +17426,163 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:I13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="9" width="13.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B2" s="79" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="82" t="s">
+        <v>102</v>
+      </c>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B3" s="66" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="66" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="66" t="s">
+        <v>136</v>
+      </c>
+      <c r="E3" s="66" t="s">
+        <v>137</v>
+      </c>
+      <c r="F3" s="66" t="s">
+        <v>98</v>
+      </c>
+      <c r="G3" s="67" t="s">
+        <v>103</v>
+      </c>
+      <c r="H3" s="67" t="s">
+        <v>104</v>
+      </c>
+      <c r="I3" s="67" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B4" s="64" t="s">
+        <v>138</v>
+      </c>
+      <c r="C4" s="64">
+        <v>2500</v>
+      </c>
+      <c r="D4" s="64">
+        <v>0.1</v>
+      </c>
+      <c r="E4" s="64">
+        <v>0.4</v>
+      </c>
+      <c r="F4" s="65"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B5" s="62"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="63"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B6" s="62"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="63"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="63"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B8" s="64"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="63"/>
+      <c r="H8" s="63"/>
+      <c r="I8" s="63"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B9" s="62"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="63"/>
+      <c r="H9" s="63"/>
+      <c r="I9" s="63"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B10" s="62"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="64"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="63"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="63"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B11" s="62"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="63"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B12" s="85"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B13" s="85"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="G2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V20"/>
   <sheetViews>
     <sheetView topLeftCell="A272" workbookViewId="0">
@@ -17647,7 +17826,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:S18"/>
   <sheetViews>

</xml_diff>

<commit_message>
Last commit b4 creating main_v2
</commit_message>
<xml_diff>
--- a/results/General Sheet.xlsx
+++ b/results/General Sheet.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="139">
   <si>
     <t>Factr Investigation</t>
   </si>
@@ -439,7 +439,7 @@
     <t>xdiv</t>
   </si>
   <si>
-    <t>case0</t>
+    <t>Case 0_results</t>
   </si>
 </sst>
 </file>
@@ -734,7 +734,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -817,6 +817,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -856,8 +859,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2648,6 +2672,365 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>error</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> vs bias</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Type2Bias!$C$6:$J$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Type2Bias!$C$8:$J$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5.7099952665768403E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.3041335786281497E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.82717324468389E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.4947721897162307E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.1371568722350499E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.8173887093831805E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1034961894986E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.22877876166556699</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-792C-4505-84EA-3B301BF496C9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="549001680"/>
+        <c:axId val="549002664"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="549001680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="549002664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="549002664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="549001680"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout>
@@ -3077,7 +3460,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -7305,6 +7688,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -9690,6 +10113,522 @@
 </file>
 
 <file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -14957,6 +15896,41 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
+      <xdr:colOff>73025</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>377825</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>101599</xdr:rowOff>
@@ -15329,17 +16303,17 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="74"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="75"/>
       <c r="J2" t="s">
         <v>11</v>
       </c>
@@ -15555,17 +16529,17 @@
     </row>
     <row r="10" spans="1:23" ht="21.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="11" spans="1:23" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="72" t="s">
+      <c r="A11" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="75"/>
-      <c r="C11" s="75"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="75"/>
-      <c r="G11" s="75"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="76"/>
+      <c r="B11" s="76"/>
+      <c r="C11" s="76"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="76"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="76"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="77"/>
       <c r="J11" t="s">
         <v>43</v>
       </c>
@@ -15900,17 +16874,17 @@
       </c>
     </row>
     <row r="23" spans="1:23" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="72" t="s">
+      <c r="A23" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="73"/>
-      <c r="C23" s="73"/>
-      <c r="D23" s="73"/>
-      <c r="E23" s="73"/>
-      <c r="F23" s="73"/>
-      <c r="G23" s="73"/>
-      <c r="H23" s="73"/>
-      <c r="I23" s="74"/>
+      <c r="B23" s="74"/>
+      <c r="C23" s="74"/>
+      <c r="D23" s="74"/>
+      <c r="E23" s="74"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="74"/>
+      <c r="H23" s="74"/>
+      <c r="I23" s="75"/>
       <c r="J23" t="s">
         <v>61</v>
       </c>
@@ -16154,17 +17128,17 @@
       <c r="H31" s="20"/>
     </row>
     <row r="32" spans="1:23" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="72" t="s">
+      <c r="A32" s="73" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="73"/>
-      <c r="C32" s="73"/>
-      <c r="D32" s="73"/>
-      <c r="E32" s="73"/>
-      <c r="F32" s="73"/>
-      <c r="G32" s="73"/>
-      <c r="H32" s="73"/>
-      <c r="I32" s="74"/>
+      <c r="B32" s="74"/>
+      <c r="C32" s="74"/>
+      <c r="D32" s="74"/>
+      <c r="E32" s="74"/>
+      <c r="F32" s="74"/>
+      <c r="G32" s="74"/>
+      <c r="H32" s="74"/>
+      <c r="I32" s="75"/>
       <c r="J32" t="s">
         <v>11</v>
       </c>
@@ -16526,17 +17500,17 @@
       <c r="H45" s="20"/>
     </row>
     <row r="46" spans="1:10" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="77" t="s">
+      <c r="A46" s="78" t="s">
         <v>82</v>
       </c>
-      <c r="B46" s="73"/>
-      <c r="C46" s="73"/>
-      <c r="D46" s="73"/>
-      <c r="E46" s="73"/>
-      <c r="F46" s="73"/>
-      <c r="G46" s="73"/>
-      <c r="H46" s="73"/>
-      <c r="I46" s="74"/>
+      <c r="B46" s="74"/>
+      <c r="C46" s="74"/>
+      <c r="D46" s="74"/>
+      <c r="E46" s="74"/>
+      <c r="F46" s="74"/>
+      <c r="G46" s="74"/>
+      <c r="H46" s="74"/>
+      <c r="I46" s="75"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="55" t="s">
@@ -16885,10 +17859,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="79" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="78"/>
+      <c r="B1" s="79"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -16921,20 +17895,20 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C7" s="79" t="s">
+      <c r="C7" s="80" t="s">
         <v>101</v>
       </c>
-      <c r="D7" s="80"/>
-      <c r="E7" s="80"/>
-      <c r="F7" s="80"/>
-      <c r="G7" s="80"/>
-      <c r="H7" s="81"/>
-      <c r="I7" s="82" t="s">
+      <c r="D7" s="81"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="81"/>
+      <c r="G7" s="81"/>
+      <c r="H7" s="82"/>
+      <c r="I7" s="83" t="s">
         <v>102</v>
       </c>
-      <c r="J7" s="83"/>
-      <c r="K7" s="83"/>
-      <c r="L7" s="83"/>
+      <c r="J7" s="84"/>
+      <c r="K7" s="84"/>
+      <c r="L7" s="84"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C8" s="66" t="s">
@@ -17426,10 +18400,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I13"/>
+  <dimension ref="B2:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17437,147 +18411,198 @@
     <col min="2" max="9" width="13.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B2" s="79" t="s">
-        <v>101</v>
-      </c>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="82" t="s">
-        <v>102</v>
-      </c>
-      <c r="H2" s="83"/>
-      <c r="I2" s="83"/>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B2" s="66" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="88" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="90"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B3" s="66" t="s">
-        <v>94</v>
-      </c>
-      <c r="C3" s="66" t="s">
         <v>95</v>
       </c>
-      <c r="D3" s="66" t="s">
+      <c r="C3" s="91">
+        <v>2500</v>
+      </c>
+      <c r="D3" s="92"/>
+      <c r="E3" s="92"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="92"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="92"/>
+      <c r="J3" s="93"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B4" s="66" t="s">
         <v>136</v>
       </c>
-      <c r="E3" s="66" t="s">
+      <c r="C4" s="91">
+        <v>0.1</v>
+      </c>
+      <c r="D4" s="92"/>
+      <c r="E4" s="92"/>
+      <c r="F4" s="92"/>
+      <c r="G4" s="92"/>
+      <c r="H4" s="92"/>
+      <c r="I4" s="92"/>
+      <c r="J4" s="93"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B5" s="66" t="s">
         <v>137</v>
       </c>
-      <c r="F3" s="66" t="s">
+      <c r="C5" s="91">
+        <v>0.4</v>
+      </c>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
+      <c r="F5" s="92"/>
+      <c r="G5" s="92"/>
+      <c r="H5" s="92"/>
+      <c r="I5" s="92"/>
+      <c r="J5" s="93"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B6" s="66" t="s">
         <v>98</v>
       </c>
-      <c r="G3" s="67" t="s">
+      <c r="C6" s="62">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D6" s="62">
+        <v>0.3</v>
+      </c>
+      <c r="E6" s="64">
+        <v>0.4</v>
+      </c>
+      <c r="F6" s="64">
+        <v>0.5</v>
+      </c>
+      <c r="G6" s="62">
+        <v>0.6</v>
+      </c>
+      <c r="H6" s="62">
+        <v>0.7</v>
+      </c>
+      <c r="I6" s="62">
+        <v>0.8</v>
+      </c>
+      <c r="J6" s="62">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B7" s="67" t="s">
         <v>103</v>
       </c>
-      <c r="H3" s="67" t="s">
+      <c r="C7" s="63">
+        <v>164.67476129531801</v>
+      </c>
+      <c r="D7" s="63">
+        <v>190.88939642906101</v>
+      </c>
+      <c r="E7" s="86">
+        <v>133.46045684814399</v>
+      </c>
+      <c r="F7" s="87">
+        <v>122.851951122283</v>
+      </c>
+      <c r="G7" s="63">
+        <v>91.901008605957003</v>
+      </c>
+      <c r="H7" s="63">
+        <v>77.341222286224294</v>
+      </c>
+      <c r="I7" s="63">
+        <v>101.304563045501</v>
+      </c>
+      <c r="J7" s="63">
+        <v>108.06644010543801</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B8" s="67" t="s">
         <v>104</v>
       </c>
-      <c r="I3" s="67" t="s">
+      <c r="C8" s="63">
+        <v>5.7099952665768403E-3</v>
+      </c>
+      <c r="D8" s="63">
+        <v>4.3041335786281497E-3</v>
+      </c>
+      <c r="E8" s="86">
+        <v>2.82717324468389E-3</v>
+      </c>
+      <c r="F8" s="86">
+        <v>8.4947721897162307E-2</v>
+      </c>
+      <c r="G8" s="63">
+        <v>2.1371568722350499E-2</v>
+      </c>
+      <c r="H8" s="63">
+        <v>9.8173887093831805E-2</v>
+      </c>
+      <c r="I8" s="63">
+        <v>1.1034961894986E-2</v>
+      </c>
+      <c r="J8" s="63">
+        <v>0.22877876166556699</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B9" s="67" t="s">
         <v>105</v>
       </c>
+      <c r="C9" s="63">
+        <v>3.74758471031367E-2</v>
+      </c>
+      <c r="D9" s="63">
+        <v>2.9115771914161301E-2</v>
+      </c>
+      <c r="E9" s="86">
+        <v>1.8396133504005499E-2</v>
+      </c>
+      <c r="F9" s="86">
+        <v>0.32531973050388102</v>
+      </c>
+      <c r="G9" s="63">
+        <v>0.122043181137584</v>
+      </c>
+      <c r="H9" s="63">
+        <v>0.34553497832471902</v>
+      </c>
+      <c r="I9" s="63">
+        <v>5.0230909480799099E-2</v>
+      </c>
+      <c r="J9" s="63">
+        <v>0.505046515618509</v>
+      </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B4" s="64" t="s">
-        <v>138</v>
-      </c>
-      <c r="C4" s="64">
-        <v>2500</v>
-      </c>
-      <c r="D4" s="64">
-        <v>0.1</v>
-      </c>
-      <c r="E4" s="64">
-        <v>0.4</v>
-      </c>
-      <c r="F4" s="65"/>
-      <c r="G4" s="63"/>
-      <c r="H4" s="63"/>
-      <c r="I4" s="63"/>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B10" s="72"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B5" s="62"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64"/>
-      <c r="G5" s="63"/>
-      <c r="H5" s="63"/>
-      <c r="I5" s="63"/>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B6" s="62"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="63"/>
-      <c r="H6" s="63"/>
-      <c r="I6" s="63"/>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B7" s="62"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="64"/>
-      <c r="G7" s="63"/>
-      <c r="H7" s="63"/>
-      <c r="I7" s="63"/>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B8" s="64"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="62"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="65"/>
-      <c r="G8" s="63"/>
-      <c r="H8" s="63"/>
-      <c r="I8" s="63"/>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B9" s="62"/>
-      <c r="C9" s="62"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="64"/>
-      <c r="F9" s="64"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="63"/>
-      <c r="I9" s="63"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B10" s="62"/>
-      <c r="C10" s="62"/>
-      <c r="D10" s="62"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="63"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="63"/>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B11" s="62"/>
-      <c r="C11" s="62"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="63"/>
-      <c r="H11" s="63"/>
-      <c r="I11" s="63"/>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B12" s="85"/>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B13" s="85"/>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B11" s="72"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="G2:I2"/>
+  <mergeCells count="4">
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -17842,13 +18867,13 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:19" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="76"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="77"/>
       <c r="F4" t="s">
         <v>11</v>
       </c>
@@ -18000,12 +19025,12 @@
       <c r="A12" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="P12" s="84" t="s">
+      <c r="P12" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="Q12" s="84"/>
-      <c r="R12" s="84"/>
-      <c r="S12" s="84"/>
+      <c r="Q12" s="85"/>
+      <c r="R12" s="85"/>
+      <c r="S12" s="85"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
@@ -18026,10 +19051,10 @@
       <c r="F13" s="16">
         <v>2.8798000000000001E-5</v>
       </c>
-      <c r="P13" s="84"/>
-      <c r="Q13" s="84"/>
-      <c r="R13" s="84"/>
-      <c r="S13" s="84"/>
+      <c r="P13" s="85"/>
+      <c r="Q13" s="85"/>
+      <c r="R13" s="85"/>
+      <c r="S13" s="85"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14" s="13" t="s">
@@ -18051,10 +19076,10 @@
       <c r="F14" s="7">
         <v>1.058E-4</v>
       </c>
-      <c r="P14" s="84"/>
-      <c r="Q14" s="84"/>
-      <c r="R14" s="84"/>
-      <c r="S14" s="84"/>
+      <c r="P14" s="85"/>
+      <c r="Q14" s="85"/>
+      <c r="R14" s="85"/>
+      <c r="S14" s="85"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15" s="13" t="s">
@@ -18074,10 +19099,10 @@
         <v>8.7702261052175406E-2</v>
       </c>
       <c r="F15" s="6"/>
-      <c r="P15" s="84"/>
-      <c r="Q15" s="84"/>
-      <c r="R15" s="84"/>
-      <c r="S15" s="84"/>
+      <c r="P15" s="85"/>
+      <c r="Q15" s="85"/>
+      <c r="R15" s="85"/>
+      <c r="S15" s="85"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16" s="14" t="s">
@@ -18099,19 +19124,19 @@
       <c r="F16" s="10">
         <v>1.1573000000000001E-5</v>
       </c>
-      <c r="P16" s="84"/>
-      <c r="Q16" s="84"/>
-      <c r="R16" s="84"/>
-      <c r="S16" s="84"/>
+      <c r="P16" s="85"/>
+      <c r="Q16" s="85"/>
+      <c r="R16" s="85"/>
+      <c r="S16" s="85"/>
     </row>
     <row r="18" spans="1:5" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="77" t="s">
+      <c r="A18" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="75"/>
-      <c r="C18" s="75"/>
-      <c r="D18" s="75"/>
-      <c r="E18" s="76"/>
+      <c r="B18" s="76"/>
+      <c r="C18" s="76"/>
+      <c r="D18" s="76"/>
+      <c r="E18" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>